<commit_message>
[CSV] Idol 정보 추가
</commit_message>
<xml_diff>
--- a/Design/Tables/Idol.xlsx
+++ b/Design/Tables/Idol.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20343"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0E6D26-2DFB-4170-B230-2B8A21059DA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04E2B41-A3F0-44A5-8BCF-AAE52A390148}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -50,15 +50,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Min</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Max</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>normal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CurMin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CurMax</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PotenMin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PotenMax</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -384,15 +396,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G2" activeCellId="1" sqref="E2 G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -400,13 +412,19 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -419,22 +437,34 @@
       <c r="D2" t="s">
         <v>1</v>
       </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>75</v>
+        <v>40</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -445,10 +475,16 @@
         <v>20</v>
       </c>
       <c r="D4">
+        <v>70</v>
+      </c>
+      <c r="E4">
+        <v>40</v>
+      </c>
+      <c r="F4">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -459,10 +495,16 @@
         <v>40</v>
       </c>
       <c r="D5">
+        <v>80</v>
+      </c>
+      <c r="E5">
+        <v>60</v>
+      </c>
+      <c r="F5">
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -473,11 +515,18 @@
         <v>60</v>
       </c>
       <c r="D6">
+        <v>95</v>
+      </c>
+      <c r="E6">
+        <v>80</v>
+      </c>
+      <c r="F6">
         <v>99</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>